<commit_message>
Update change mysql table name to upper case.xlsx
change text_data to biog_text_data and add other table names
</commit_message>
<xml_diff>
--- a/change mysql table name to upper case.xlsx
+++ b/change mysql table name to upper case.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hongsu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\git_projects\accessAndMySQLTransfer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8393B90-2EDC-411C-B0B6-D1C238551B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7677AA0-6E95-4F36-9795-D98EFCE02B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50C32DAB-0FA3-4A6C-8155-BE0701969030}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>TableName</t>
   </si>
@@ -263,9 +263,6 @@
     <t>TEXT_CODES</t>
   </si>
   <si>
-    <t>TEXT_DATA</t>
-  </si>
-  <si>
     <t>TEXT_ROLE_CODES</t>
   </si>
   <si>
@@ -276,6 +273,24 @@
   </si>
   <si>
     <t>TEXT_INSTANCE_DATA</t>
+  </si>
+  <si>
+    <t>BIOG_TEXT_DATA</t>
+  </si>
+  <si>
+    <t>INDEXYEAR_TYPE_CODES</t>
+  </si>
+  <si>
+    <t>FORMLABELS</t>
+  </si>
+  <si>
+    <t>COPYMISSINGTABLES</t>
+  </si>
+  <si>
+    <t>COPYTABLES</t>
+  </si>
+  <si>
+    <t>COPYTABLESDEFAULT</t>
   </si>
 </sst>
 </file>
@@ -315,7 +330,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -353,17 +368,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -681,15 +714,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D29AFA-D650-4719-BE04-0F79161E8DDB}">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="1" max="1" width="39.21875" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -707,7 +740,7 @@
         <v>addr_belongs_data</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C55" si="0">"ALTER TABLE "&amp;B2&amp;" RENAME TO "&amp;A2&amp;";"</f>
+        <f>"ALTER TABLE "&amp;B2&amp;" RENAME TO "&amp;A2&amp;";"</f>
         <v>ALTER TABLE addr_belongs_data RENAME TO ADDR_BELONGS_DATA;</v>
       </c>
     </row>
@@ -716,11 +749,11 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B66" si="1">LOWER(A3)</f>
+        <f>LOWER(A3)</f>
         <v>addr_codes</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B3&amp;" RENAME TO "&amp;A3&amp;";"</f>
         <v>ALTER TABLE addr_codes RENAME TO ADDR_CODES;</v>
       </c>
     </row>
@@ -729,11 +762,11 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A4)</f>
         <v>addresses</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B4&amp;" RENAME TO "&amp;A4&amp;";"</f>
         <v>ALTER TABLE addresses RENAME TO ADDRESSES;</v>
       </c>
     </row>
@@ -742,11 +775,11 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A5)</f>
         <v>altname_codes</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B5&amp;" RENAME TO "&amp;A5&amp;";"</f>
         <v>ALTER TABLE altname_codes RENAME TO ALTNAME_CODES;</v>
       </c>
     </row>
@@ -755,11 +788,11 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A6)</f>
         <v>altname_data</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B6&amp;" RENAME TO "&amp;A6&amp;";"</f>
         <v>ALTER TABLE altname_data RENAME TO ALTNAME_DATA;</v>
       </c>
     </row>
@@ -768,11 +801,11 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A7)</f>
         <v>appointment_type_codes</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B7&amp;" RENAME TO "&amp;A7&amp;";"</f>
         <v>ALTER TABLE appointment_type_codes RENAME TO APPOINTMENT_TYPE_CODES;</v>
       </c>
     </row>
@@ -781,11 +814,11 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A8)</f>
         <v>assoc_code_type_rel</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B8&amp;" RENAME TO "&amp;A8&amp;";"</f>
         <v>ALTER TABLE assoc_code_type_rel RENAME TO ASSOC_CODE_TYPE_REL;</v>
       </c>
     </row>
@@ -794,11 +827,11 @@
         <v>8</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A9)</f>
         <v>assoc_codes</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B9&amp;" RENAME TO "&amp;A9&amp;";"</f>
         <v>ALTER TABLE assoc_codes RENAME TO ASSOC_CODES;</v>
       </c>
     </row>
@@ -807,11 +840,11 @@
         <v>9</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A10)</f>
         <v>assoc_data</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B10&amp;" RENAME TO "&amp;A10&amp;";"</f>
         <v>ALTER TABLE assoc_data RENAME TO ASSOC_DATA;</v>
       </c>
     </row>
@@ -820,11 +853,11 @@
         <v>10</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A11)</f>
         <v>assoc_types</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B11&amp;" RENAME TO "&amp;A11&amp;";"</f>
         <v>ALTER TABLE assoc_types RENAME TO ASSOC_TYPES;</v>
       </c>
     </row>
@@ -833,11 +866,11 @@
         <v>11</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A12)</f>
         <v>assume_office_codes</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B12&amp;" RENAME TO "&amp;A12&amp;";"</f>
         <v>ALTER TABLE assume_office_codes RENAME TO ASSUME_OFFICE_CODES;</v>
       </c>
     </row>
@@ -846,11 +879,11 @@
         <v>12</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A13)</f>
         <v>biog_addr_codes</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B13&amp;" RENAME TO "&amp;A13&amp;";"</f>
         <v>ALTER TABLE biog_addr_codes RENAME TO BIOG_ADDR_CODES;</v>
       </c>
     </row>
@@ -859,11 +892,11 @@
         <v>13</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A14)</f>
         <v>biog_addr_data</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B14&amp;" RENAME TO "&amp;A14&amp;";"</f>
         <v>ALTER TABLE biog_addr_data RENAME TO BIOG_ADDR_DATA;</v>
       </c>
     </row>
@@ -872,11 +905,11 @@
         <v>14</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A15)</f>
         <v>biog_inst_codes</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B15&amp;" RENAME TO "&amp;A15&amp;";"</f>
         <v>ALTER TABLE biog_inst_codes RENAME TO BIOG_INST_CODES;</v>
       </c>
     </row>
@@ -885,11 +918,11 @@
         <v>15</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A16)</f>
         <v>biog_inst_data</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B16&amp;" RENAME TO "&amp;A16&amp;";"</f>
         <v>ALTER TABLE biog_inst_data RENAME TO BIOG_INST_DATA;</v>
       </c>
     </row>
@@ -898,11 +931,11 @@
         <v>16</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A17)</f>
         <v>biog_main</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B17&amp;" RENAME TO "&amp;A17&amp;";"</f>
         <v>ALTER TABLE biog_main RENAME TO BIOG_MAIN;</v>
       </c>
     </row>
@@ -911,834 +944,902 @@
         <v>17</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="1"/>
+        <f>LOWER(A18)</f>
         <v>biog_source_data</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="0"/>
+        <f>"ALTER TABLE "&amp;B18&amp;" RENAME TO "&amp;A18&amp;";"</f>
         <v>ALTER TABLE biog_source_data RENAME TO BIOG_SOURCE_DATA;</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="1"/>
-        <v>choronym_codes</v>
+        <f>LOWER(A19)</f>
+        <v>biog_text_data</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE choronym_codes RENAME TO CHORONYM_CODES;</v>
+        <f>"ALTER TABLE "&amp;B19&amp;" RENAME TO "&amp;A19&amp;";"</f>
+        <v>ALTER TABLE biog_text_data RENAME TO BIOG_TEXT_DATA;</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="1"/>
-        <v>country_codes</v>
+        <f>LOWER(A20)</f>
+        <v>choronym_codes</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE country_codes RENAME TO COUNTRY_CODES;</v>
+        <f>"ALTER TABLE "&amp;B20&amp;" RENAME TO "&amp;A20&amp;";"</f>
+        <v>ALTER TABLE choronym_codes RENAME TO CHORONYM_CODES;</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>20</v>
+      <c r="A21" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="1"/>
-        <v>database_link_codes</v>
+        <f>LOWER(A21)</f>
+        <v>copymissingtables</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE database_link_codes RENAME TO DATABASE_LINK_CODES;</v>
+        <f>"ALTER TABLE "&amp;B21&amp;" RENAME TO "&amp;A21&amp;";"</f>
+        <v>ALTER TABLE copymissingtables RENAME TO COPYMISSINGTABLES;</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
+      <c r="A22" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="1"/>
-        <v>database_link_data</v>
+        <f>LOWER(A22)</f>
+        <v>copytables</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE database_link_data RENAME TO DATABASE_LINK_DATA;</v>
+        <f>"ALTER TABLE "&amp;B22&amp;" RENAME TO "&amp;A22&amp;";"</f>
+        <v>ALTER TABLE copytables RENAME TO COPYTABLES;</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
+      <c r="A23" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="1"/>
-        <v>dynasties</v>
+        <f>LOWER(A23)</f>
+        <v>copytablesdefault</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE dynasties RENAME TO DYNASTIES;</v>
+        <f>"ALTER TABLE "&amp;B23&amp;" RENAME TO "&amp;A23&amp;";"</f>
+        <v>ALTER TABLE copytablesdefault RENAME TO COPYTABLESDEFAULT;</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="1"/>
-        <v>entry_code_type_rel</v>
+        <f>LOWER(A24)</f>
+        <v>country_codes</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE entry_code_type_rel RENAME TO ENTRY_CODE_TYPE_REL;</v>
+        <f>"ALTER TABLE "&amp;B24&amp;" RENAME TO "&amp;A24&amp;";"</f>
+        <v>ALTER TABLE country_codes RENAME TO COUNTRY_CODES;</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="1"/>
-        <v>entry_codes</v>
+        <f>LOWER(A25)</f>
+        <v>database_link_codes</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE entry_codes RENAME TO ENTRY_CODES;</v>
+        <f>"ALTER TABLE "&amp;B25&amp;" RENAME TO "&amp;A25&amp;";"</f>
+        <v>ALTER TABLE database_link_codes RENAME TO DATABASE_LINK_CODES;</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="1"/>
-        <v>entry_data</v>
+        <f>LOWER(A26)</f>
+        <v>database_link_data</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE entry_data RENAME TO ENTRY_DATA;</v>
+        <f>"ALTER TABLE "&amp;B26&amp;" RENAME TO "&amp;A26&amp;";"</f>
+        <v>ALTER TABLE database_link_data RENAME TO DATABASE_LINK_DATA;</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="1"/>
-        <v>entry_types</v>
+        <f>LOWER(A27)</f>
+        <v>dynasties</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE entry_types RENAME TO ENTRY_TYPES;</v>
+        <f>"ALTER TABLE "&amp;B27&amp;" RENAME TO "&amp;A27&amp;";"</f>
+        <v>ALTER TABLE dynasties RENAME TO DYNASTIES;</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="1"/>
-        <v>ethnicity_tribe_codes</v>
+        <f>LOWER(A28)</f>
+        <v>entry_code_type_rel</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE ethnicity_tribe_codes RENAME TO ETHNICITY_TRIBE_CODES;</v>
+        <f>"ALTER TABLE "&amp;B28&amp;" RENAME TO "&amp;A28&amp;";"</f>
+        <v>ALTER TABLE entry_code_type_rel RENAME TO ENTRY_CODE_TYPE_REL;</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="1"/>
-        <v>event_codes</v>
+        <f>LOWER(A29)</f>
+        <v>entry_codes</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE event_codes RENAME TO EVENT_CODES;</v>
+        <f>"ALTER TABLE "&amp;B29&amp;" RENAME TO "&amp;A29&amp;";"</f>
+        <v>ALTER TABLE entry_codes RENAME TO ENTRY_CODES;</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="1"/>
-        <v>events_addr</v>
+        <f>LOWER(A30)</f>
+        <v>entry_data</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE events_addr RENAME TO EVENTS_ADDR;</v>
+        <f>"ALTER TABLE "&amp;B30&amp;" RENAME TO "&amp;A30&amp;";"</f>
+        <v>ALTER TABLE entry_data RENAME TO ENTRY_DATA;</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="1"/>
-        <v>events_data</v>
+        <f>LOWER(A31)</f>
+        <v>entry_types</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE events_data RENAME TO EVENTS_DATA;</v>
+        <f>"ALTER TABLE "&amp;B31&amp;" RENAME TO "&amp;A31&amp;";"</f>
+        <v>ALTER TABLE entry_types RENAME TO ENTRY_TYPES;</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="1"/>
-        <v>extant_codes</v>
+        <f>LOWER(A32)</f>
+        <v>ethnicity_tribe_codes</v>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE extant_codes RENAME TO EXTANT_CODES;</v>
+        <f>"ALTER TABLE "&amp;B32&amp;" RENAME TO "&amp;A32&amp;";"</f>
+        <v>ALTER TABLE ethnicity_tribe_codes RENAME TO ETHNICITY_TRIBE_CODES;</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="1"/>
-        <v>foreignkeys</v>
+        <f>LOWER(A33)</f>
+        <v>event_codes</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE foreignkeys RENAME TO FOREIGNKEYS;</v>
+        <f>"ALTER TABLE "&amp;B33&amp;" RENAME TO "&amp;A33&amp;";"</f>
+        <v>ALTER TABLE event_codes RENAME TO EVENT_CODES;</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="1"/>
-        <v>ganzhi_codes</v>
+        <f>LOWER(A34)</f>
+        <v>events_addr</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE ganzhi_codes RENAME TO GANZHI_CODES;</v>
+        <f>"ALTER TABLE "&amp;B34&amp;" RENAME TO "&amp;A34&amp;";"</f>
+        <v>ALTER TABLE events_addr RENAME TO EVENTS_ADDR;</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="1"/>
-        <v>household_status_codes</v>
+        <f>LOWER(A35)</f>
+        <v>events_data</v>
       </c>
       <c r="C35" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE household_status_codes RENAME TO HOUSEHOLD_STATUS_CODES;</v>
+        <f>"ALTER TABLE "&amp;B35&amp;" RENAME TO "&amp;A35&amp;";"</f>
+        <v>ALTER TABLE events_data RENAME TO EVENTS_DATA;</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="1"/>
-        <v>kin_data</v>
+        <f>LOWER(A36)</f>
+        <v>extant_codes</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE kin_data RENAME TO KIN_DATA;</v>
+        <f>"ALTER TABLE "&amp;B36&amp;" RENAME TO "&amp;A36&amp;";"</f>
+        <v>ALTER TABLE extant_codes RENAME TO EXTANT_CODES;</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" si="1"/>
-        <v>kin_mourning</v>
+        <f>LOWER(A37)</f>
+        <v>foreignkeys</v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE kin_mourning RENAME TO KIN_MOURNING;</v>
+        <f>"ALTER TABLE "&amp;B37&amp;" RENAME TO "&amp;A37&amp;";"</f>
+        <v>ALTER TABLE foreignkeys RENAME TO FOREIGNKEYS;</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" si="1"/>
-        <v>kin_mourning_steps</v>
+        <f>LOWER(A38)</f>
+        <v>formlabels</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE kin_mourning_steps RENAME TO KIN_MOURNING_STEPS;</v>
+        <f>"ALTER TABLE "&amp;B38&amp;" RENAME TO "&amp;A38&amp;";"</f>
+        <v>ALTER TABLE formlabels RENAME TO FORMLABELS;</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" si="1"/>
-        <v>kinship_codes</v>
+        <f>LOWER(A39)</f>
+        <v>ganzhi_codes</v>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE kinship_codes RENAME TO KINSHIP_CODES;</v>
+        <f>"ALTER TABLE "&amp;B39&amp;" RENAME TO "&amp;A39&amp;";"</f>
+        <v>ALTER TABLE ganzhi_codes RENAME TO GANZHI_CODES;</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="1"/>
-        <v>literarygenre_codes</v>
+        <f>LOWER(A40)</f>
+        <v>household_status_codes</v>
       </c>
       <c r="C40" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE literarygenre_codes RENAME TO LITERARYGENRE_CODES;</v>
+        <f>"ALTER TABLE "&amp;B40&amp;" RENAME TO "&amp;A40&amp;";"</f>
+        <v>ALTER TABLE household_status_codes RENAME TO HOUSEHOLD_STATUS_CODES;</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="1"/>
-        <v>measure_codes</v>
+        <f>LOWER(A41)</f>
+        <v>indexyear_type_codes</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE measure_codes RENAME TO MEASURE_CODES;</v>
+        <f>"ALTER TABLE "&amp;B41&amp;" RENAME TO "&amp;A41&amp;";"</f>
+        <v>ALTER TABLE indexyear_type_codes RENAME TO INDEXYEAR_TYPE_CODES;</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="1"/>
-        <v>nian_hao</v>
+        <f>LOWER(A42)</f>
+        <v>kin_data</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE nian_hao RENAME TO NIAN_HAO;</v>
+        <f>"ALTER TABLE "&amp;B42&amp;" RENAME TO "&amp;A42&amp;";"</f>
+        <v>ALTER TABLE kin_data RENAME TO KIN_DATA;</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="1"/>
-        <v>occasion_codes</v>
+        <f>LOWER(A43)</f>
+        <v>kin_mourning</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE occasion_codes RENAME TO OCCASION_CODES;</v>
+        <f>"ALTER TABLE "&amp;B43&amp;" RENAME TO "&amp;A43&amp;";"</f>
+        <v>ALTER TABLE kin_mourning RENAME TO KIN_MOURNING;</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="1"/>
-        <v>office_categories</v>
+        <f>LOWER(A44)</f>
+        <v>kin_mourning_steps</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE office_categories RENAME TO OFFICE_CATEGORIES;</v>
+        <f>"ALTER TABLE "&amp;B44&amp;" RENAME TO "&amp;A44&amp;";"</f>
+        <v>ALTER TABLE kin_mourning_steps RENAME TO KIN_MOURNING_STEPS;</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="1"/>
-        <v>office_code_type_rel</v>
+        <f>LOWER(A45)</f>
+        <v>kinship_codes</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE office_code_type_rel RENAME TO OFFICE_CODE_TYPE_REL;</v>
+        <f>"ALTER TABLE "&amp;B45&amp;" RENAME TO "&amp;A45&amp;";"</f>
+        <v>ALTER TABLE kinship_codes RENAME TO KINSHIP_CODES;</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B46" t="str">
-        <f t="shared" si="1"/>
-        <v>office_codes</v>
+        <f>LOWER(A46)</f>
+        <v>literarygenre_codes</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE office_codes RENAME TO OFFICE_CODES;</v>
+        <f>"ALTER TABLE "&amp;B46&amp;" RENAME TO "&amp;A46&amp;";"</f>
+        <v>ALTER TABLE literarygenre_codes RENAME TO LITERARYGENRE_CODES;</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B47" t="str">
-        <f t="shared" si="1"/>
-        <v>office_codes_conversion</v>
+        <f>LOWER(A47)</f>
+        <v>measure_codes</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE office_codes_conversion RENAME TO OFFICE_CODES_CONVERSION;</v>
+        <f>"ALTER TABLE "&amp;B47&amp;" RENAME TO "&amp;A47&amp;";"</f>
+        <v>ALTER TABLE measure_codes RENAME TO MEASURE_CODES;</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B48" t="str">
-        <f t="shared" si="1"/>
-        <v>office_type_tree</v>
+        <f>LOWER(A48)</f>
+        <v>nian_hao</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE office_type_tree RENAME TO OFFICE_TYPE_TREE;</v>
+        <f>"ALTER TABLE "&amp;B48&amp;" RENAME TO "&amp;A48&amp;";"</f>
+        <v>ALTER TABLE nian_hao RENAME TO NIAN_HAO;</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" si="1"/>
-        <v>office_type_tree_backup</v>
+        <f>LOWER(A49)</f>
+        <v>occasion_codes</v>
       </c>
       <c r="C49" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE office_type_tree_backup RENAME TO OFFICE_TYPE_TREE_BACKUP;</v>
+        <f>"ALTER TABLE "&amp;B49&amp;" RENAME TO "&amp;A49&amp;";"</f>
+        <v>ALTER TABLE occasion_codes RENAME TO OCCASION_CODES;</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B50" t="str">
-        <f t="shared" si="1"/>
-        <v>parental_status_codes</v>
+        <f>LOWER(A50)</f>
+        <v>office_categories</v>
       </c>
       <c r="C50" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE parental_status_codes RENAME TO PARENTAL_STATUS_CODES;</v>
+        <f>"ALTER TABLE "&amp;B50&amp;" RENAME TO "&amp;A50&amp;";"</f>
+        <v>ALTER TABLE office_categories RENAME TO OFFICE_CATEGORIES;</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B51" t="str">
-        <f t="shared" si="1"/>
-        <v>place_codes</v>
+        <f>LOWER(A51)</f>
+        <v>office_code_type_rel</v>
       </c>
       <c r="C51" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE place_codes RENAME TO PLACE_CODES;</v>
+        <f>"ALTER TABLE "&amp;B51&amp;" RENAME TO "&amp;A51&amp;";"</f>
+        <v>ALTER TABLE office_code_type_rel RENAME TO OFFICE_CODE_TYPE_REL;</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B52" t="str">
-        <f t="shared" si="1"/>
-        <v>possession_act_codes</v>
+        <f>LOWER(A52)</f>
+        <v>office_codes</v>
       </c>
       <c r="C52" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE possession_act_codes RENAME TO POSSESSION_ACT_CODES;</v>
+        <f>"ALTER TABLE "&amp;B52&amp;" RENAME TO "&amp;A52&amp;";"</f>
+        <v>ALTER TABLE office_codes RENAME TO OFFICE_CODES;</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B53" t="str">
-        <f t="shared" si="1"/>
-        <v>possession_addr</v>
+        <f>LOWER(A53)</f>
+        <v>office_codes_conversion</v>
       </c>
       <c r="C53" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE possession_addr RENAME TO POSSESSION_ADDR;</v>
+        <f>"ALTER TABLE "&amp;B53&amp;" RENAME TO "&amp;A53&amp;";"</f>
+        <v>ALTER TABLE office_codes_conversion RENAME TO OFFICE_CODES_CONVERSION;</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B54" t="str">
-        <f t="shared" si="1"/>
-        <v>possession_data</v>
+        <f>LOWER(A54)</f>
+        <v>office_type_tree</v>
       </c>
       <c r="C54" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE possession_data RENAME TO POSSESSION_DATA;</v>
+        <f>"ALTER TABLE "&amp;B54&amp;" RENAME TO "&amp;A54&amp;";"</f>
+        <v>ALTER TABLE office_type_tree RENAME TO OFFICE_TYPE_TREE;</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B55" t="str">
-        <f t="shared" si="1"/>
-        <v>posted_to_addr_data</v>
+        <f>LOWER(A55)</f>
+        <v>office_type_tree_backup</v>
       </c>
       <c r="C55" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE posted_to_addr_data RENAME TO POSTED_TO_ADDR_DATA;</v>
+        <f>"ALTER TABLE "&amp;B55&amp;" RENAME TO "&amp;A55&amp;";"</f>
+        <v>ALTER TABLE office_type_tree_backup RENAME TO OFFICE_TYPE_TREE_BACKUP;</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" si="1"/>
-        <v>posted_to_office_data</v>
+        <f>LOWER(A56)</f>
+        <v>parental_status_codes</v>
       </c>
       <c r="C56" t="str">
         <f>"ALTER TABLE "&amp;B56&amp;" RENAME TO "&amp;A56&amp;";"</f>
-        <v>ALTER TABLE posted_to_office_data RENAME TO POSTED_TO_OFFICE_DATA;</v>
+        <v>ALTER TABLE parental_status_codes RENAME TO PARENTAL_STATUS_CODES;</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B57" t="str">
-        <f t="shared" si="1"/>
-        <v>posting_data</v>
+        <f>LOWER(A57)</f>
+        <v>place_codes</v>
       </c>
       <c r="C57" t="str">
-        <f t="shared" ref="C57:C81" si="2">"ALTER TABLE "&amp;B57&amp;" RENAME TO "&amp;A57&amp;";"</f>
-        <v>ALTER TABLE posting_data RENAME TO POSTING_DATA;</v>
+        <f>"ALTER TABLE "&amp;B57&amp;" RENAME TO "&amp;A57&amp;";"</f>
+        <v>ALTER TABLE place_codes RENAME TO PLACE_CODES;</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B58" t="str">
-        <f t="shared" si="1"/>
-        <v>scholarlytopic_codes</v>
+        <f>LOWER(A58)</f>
+        <v>possession_act_codes</v>
       </c>
       <c r="C58" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE scholarlytopic_codes RENAME TO SCHOLARLYTOPIC_CODES;</v>
+        <f>"ALTER TABLE "&amp;B58&amp;" RENAME TO "&amp;A58&amp;";"</f>
+        <v>ALTER TABLE possession_act_codes RENAME TO POSSESSION_ACT_CODES;</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" si="1"/>
-        <v>social_institution_addr</v>
+        <f>LOWER(A59)</f>
+        <v>possession_addr</v>
       </c>
       <c r="C59" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE social_institution_addr RENAME TO SOCIAL_INSTITUTION_ADDR;</v>
+        <f>"ALTER TABLE "&amp;B59&amp;" RENAME TO "&amp;A59&amp;";"</f>
+        <v>ALTER TABLE possession_addr RENAME TO POSSESSION_ADDR;</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" si="1"/>
-        <v>social_institution_addr_types</v>
+        <f>LOWER(A60)</f>
+        <v>possession_data</v>
       </c>
       <c r="C60" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE social_institution_addr_types RENAME TO SOCIAL_INSTITUTION_ADDR_TYPES;</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <f>"ALTER TABLE "&amp;B60&amp;" RENAME TO "&amp;A60&amp;";"</f>
+        <v>ALTER TABLE possession_data RENAME TO POSSESSION_DATA;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="1"/>
-        <v>social_institution_altname_codes</v>
+        <f>LOWER(A61)</f>
+        <v>posted_to_addr_data</v>
       </c>
       <c r="C61" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE social_institution_altname_codes RENAME TO SOCIAL_INSTITUTION_ALTNAME_CODES;</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <f>"ALTER TABLE "&amp;B61&amp;" RENAME TO "&amp;A61&amp;";"</f>
+        <v>ALTER TABLE posted_to_addr_data RENAME TO POSTED_TO_ADDR_DATA;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="1"/>
-        <v>social_institution_altname_data</v>
+        <f>LOWER(A62)</f>
+        <v>posted_to_office_data</v>
       </c>
       <c r="C62" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE social_institution_altname_data RENAME TO SOCIAL_INSTITUTION_ALTNAME_DATA;</v>
+        <f>"ALTER TABLE "&amp;B62&amp;" RENAME TO "&amp;A62&amp;";"</f>
+        <v>ALTER TABLE posted_to_office_data RENAME TO POSTED_TO_OFFICE_DATA;</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" si="1"/>
-        <v>social_institution_codes</v>
+        <f>LOWER(A63)</f>
+        <v>posting_data</v>
       </c>
       <c r="C63" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE social_institution_codes RENAME TO SOCIAL_INSTITUTION_CODES;</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <f>"ALTER TABLE "&amp;B63&amp;" RENAME TO "&amp;A63&amp;";"</f>
+        <v>ALTER TABLE posting_data RENAME TO POSTING_DATA;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="1"/>
-        <v>social_institution_codes_conversion</v>
+        <f>LOWER(A64)</f>
+        <v>scholarlytopic_codes</v>
       </c>
       <c r="C64" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE social_institution_codes_conversion RENAME TO SOCIAL_INSTITUTION_CODES_CONVERSION;</v>
+        <f>"ALTER TABLE "&amp;B64&amp;" RENAME TO "&amp;A64&amp;";"</f>
+        <v>ALTER TABLE scholarlytopic_codes RENAME TO SCHOLARLYTOPIC_CODES;</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" si="1"/>
-        <v>social_institution_name_codes</v>
+        <f>LOWER(A65)</f>
+        <v>social_institution_addr</v>
       </c>
       <c r="C65" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE social_institution_name_codes RENAME TO SOCIAL_INSTITUTION_NAME_CODES;</v>
+        <f>"ALTER TABLE "&amp;B65&amp;" RENAME TO "&amp;A65&amp;";"</f>
+        <v>ALTER TABLE social_institution_addr RENAME TO SOCIAL_INSTITUTION_ADDR;</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" si="1"/>
-        <v>social_institution_types</v>
+        <f>LOWER(A66)</f>
+        <v>social_institution_addr_types</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE social_institution_types RENAME TO SOCIAL_INSTITUTION_TYPES;</v>
+        <f>"ALTER TABLE "&amp;B66&amp;" RENAME TO "&amp;A66&amp;";"</f>
+        <v>ALTER TABLE social_institution_addr_types RENAME TO SOCIAL_INSTITUTION_ADDR_TYPES;</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B81" si="3">LOWER(A67)</f>
-        <v>status_code_type_rel</v>
+        <f>LOWER(A67)</f>
+        <v>social_institution_altname_codes</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE status_code_type_rel RENAME TO STATUS_CODE_TYPE_REL;</v>
+        <f>"ALTER TABLE "&amp;B67&amp;" RENAME TO "&amp;A67&amp;";"</f>
+        <v>ALTER TABLE social_institution_altname_codes RENAME TO SOCIAL_INSTITUTION_ALTNAME_CODES;</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="3"/>
-        <v>status_codes</v>
+        <f>LOWER(A68)</f>
+        <v>social_institution_altname_data</v>
       </c>
       <c r="C68" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE status_codes RENAME TO STATUS_CODES;</v>
+        <f>"ALTER TABLE "&amp;B68&amp;" RENAME TO "&amp;A68&amp;";"</f>
+        <v>ALTER TABLE social_institution_altname_data RENAME TO SOCIAL_INSTITUTION_ALTNAME_DATA;</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="3"/>
-        <v>status_data</v>
+        <f>LOWER(A69)</f>
+        <v>social_institution_codes</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE status_data RENAME TO STATUS_DATA;</v>
+        <f>"ALTER TABLE "&amp;B69&amp;" RENAME TO "&amp;A69&amp;";"</f>
+        <v>ALTER TABLE social_institution_codes RENAME TO SOCIAL_INSTITUTION_CODES;</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="3"/>
-        <v>status_types</v>
+        <f>LOWER(A70)</f>
+        <v>social_institution_codes_conversion</v>
       </c>
       <c r="C70" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE status_types RENAME TO STATUS_TYPES;</v>
+        <f>"ALTER TABLE "&amp;B70&amp;" RENAME TO "&amp;A70&amp;";"</f>
+        <v>ALTER TABLE social_institution_codes_conversion RENAME TO SOCIAL_INSTITUTION_CODES_CONVERSION;</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="3"/>
-        <v>tablesfields</v>
+        <f>LOWER(A71)</f>
+        <v>social_institution_name_codes</v>
       </c>
       <c r="C71" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE tablesfields RENAME TO TABLESFIELDS;</v>
+        <f>"ALTER TABLE "&amp;B71&amp;" RENAME TO "&amp;A71&amp;";"</f>
+        <v>ALTER TABLE social_institution_name_codes RENAME TO SOCIAL_INSTITUTION_NAME_CODES;</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="3"/>
-        <v>tablesfieldschanges</v>
+        <f>LOWER(A72)</f>
+        <v>social_institution_types</v>
       </c>
       <c r="C72" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE tablesfieldschanges RENAME TO TABLESFIELDSCHANGES;</v>
+        <f>"ALTER TABLE "&amp;B72&amp;" RENAME TO "&amp;A72&amp;";"</f>
+        <v>ALTER TABLE social_institution_types RENAME TO SOCIAL_INSTITUTION_TYPES;</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="3"/>
-        <v>text_biblcat_code_type_rel</v>
+        <f>LOWER(A73)</f>
+        <v>status_code_type_rel</v>
       </c>
       <c r="C73" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE text_biblcat_code_type_rel RENAME TO TEXT_BIBLCAT_CODE_TYPE_REL;</v>
+        <f>"ALTER TABLE "&amp;B73&amp;" RENAME TO "&amp;A73&amp;";"</f>
+        <v>ALTER TABLE status_code_type_rel RENAME TO STATUS_CODE_TYPE_REL;</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B74" t="str">
-        <f t="shared" si="3"/>
-        <v>text_biblcat_codes</v>
+        <f>LOWER(A74)</f>
+        <v>status_codes</v>
       </c>
       <c r="C74" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE text_biblcat_codes RENAME TO TEXT_BIBLCAT_CODES;</v>
+        <f>"ALTER TABLE "&amp;B74&amp;" RENAME TO "&amp;A74&amp;";"</f>
+        <v>ALTER TABLE status_codes RENAME TO STATUS_CODES;</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B75" t="str">
-        <f t="shared" si="3"/>
-        <v>text_biblcat_types</v>
+        <f>LOWER(A75)</f>
+        <v>status_data</v>
       </c>
       <c r="C75" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE text_biblcat_types RENAME TO TEXT_BIBLCAT_TYPES;</v>
+        <f>"ALTER TABLE "&amp;B75&amp;" RENAME TO "&amp;A75&amp;";"</f>
+        <v>ALTER TABLE status_data RENAME TO STATUS_DATA;</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B76" t="str">
-        <f t="shared" si="3"/>
-        <v>text_codes</v>
+        <f>LOWER(A76)</f>
+        <v>status_types</v>
       </c>
       <c r="C76" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE text_codes RENAME TO TEXT_CODES;</v>
+        <f>"ALTER TABLE "&amp;B76&amp;" RENAME TO "&amp;A76&amp;";"</f>
+        <v>ALTER TABLE status_types RENAME TO STATUS_TYPES;</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B77" t="str">
-        <f t="shared" si="3"/>
-        <v>text_data</v>
+        <f>LOWER(A77)</f>
+        <v>tablesfields</v>
       </c>
       <c r="C77" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE text_data RENAME TO TEXT_DATA;</v>
+        <f>"ALTER TABLE "&amp;B77&amp;" RENAME TO "&amp;A77&amp;";"</f>
+        <v>ALTER TABLE tablesfields RENAME TO TABLESFIELDS;</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B78" t="str">
-        <f t="shared" si="3"/>
-        <v>text_instance_data</v>
+        <f>LOWER(A78)</f>
+        <v>tablesfieldschanges</v>
       </c>
       <c r="C78" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE text_instance_data RENAME TO TEXT_INSTANCE_DATA;</v>
+        <f>"ALTER TABLE "&amp;B78&amp;" RENAME TO "&amp;A78&amp;";"</f>
+        <v>ALTER TABLE tablesfieldschanges RENAME TO TABLESFIELDSCHANGES;</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B79" t="str">
-        <f t="shared" si="3"/>
-        <v>text_role_codes</v>
+        <f>LOWER(A79)</f>
+        <v>text_biblcat_code_type_rel</v>
       </c>
       <c r="C79" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE text_role_codes RENAME TO TEXT_ROLE_CODES;</v>
+        <f>"ALTER TABLE "&amp;B79&amp;" RENAME TO "&amp;A79&amp;";"</f>
+        <v>ALTER TABLE text_biblcat_code_type_rel RENAME TO TEXT_BIBLCAT_CODE_TYPE_REL;</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B80" t="str">
-        <f t="shared" si="3"/>
-        <v>text_type</v>
+        <f>LOWER(A80)</f>
+        <v>text_biblcat_codes</v>
       </c>
       <c r="C80" t="str">
-        <f t="shared" si="2"/>
-        <v>ALTER TABLE text_type RENAME TO TEXT_TYPE;</v>
+        <f>"ALTER TABLE "&amp;B80&amp;" RENAME TO "&amp;A80&amp;";"</f>
+        <v>ALTER TABLE text_biblcat_codes RENAME TO TEXT_BIBLCAT_CODES;</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B81" t="str">
+        <f>LOWER(A81)</f>
+        <v>text_biblcat_types</v>
+      </c>
+      <c r="C81" t="str">
+        <f>"ALTER TABLE "&amp;B81&amp;" RENAME TO "&amp;A81&amp;";"</f>
+        <v>ALTER TABLE text_biblcat_types RENAME TO TEXT_BIBLCAT_TYPES;</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B82" t="str">
+        <f>LOWER(A82)</f>
+        <v>text_codes</v>
+      </c>
+      <c r="C82" t="str">
+        <f>"ALTER TABLE "&amp;B82&amp;" RENAME TO "&amp;A82&amp;";"</f>
+        <v>ALTER TABLE text_codes RENAME TO TEXT_CODES;</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B81" t="str">
-        <f t="shared" si="3"/>
+      <c r="B83" t="str">
+        <f>LOWER(A83)</f>
+        <v>text_instance_data</v>
+      </c>
+      <c r="C83" t="str">
+        <f>"ALTER TABLE "&amp;B83&amp;" RENAME TO "&amp;A83&amp;";"</f>
+        <v>ALTER TABLE text_instance_data RENAME TO TEXT_INSTANCE_DATA;</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B84" t="str">
+        <f>LOWER(A84)</f>
+        <v>text_role_codes</v>
+      </c>
+      <c r="C84" t="str">
+        <f>"ALTER TABLE "&amp;B84&amp;" RENAME TO "&amp;A84&amp;";"</f>
+        <v>ALTER TABLE text_role_codes RENAME TO TEXT_ROLE_CODES;</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B85" t="str">
+        <f>LOWER(A85)</f>
+        <v>text_type</v>
+      </c>
+      <c r="C85" t="str">
+        <f>"ALTER TABLE "&amp;B85&amp;" RENAME TO "&amp;A85&amp;";"</f>
+        <v>ALTER TABLE text_type RENAME TO TEXT_TYPE;</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86" t="str">
+        <f>LOWER(A86)</f>
         <v>year_range_codes</v>
       </c>
-      <c r="C81" t="str">
-        <f t="shared" si="2"/>
+      <c r="C86" t="str">
+        <f>"ALTER TABLE "&amp;B86&amp;" RENAME TO "&amp;A86&amp;";"</f>
         <v>ALTER TABLE year_range_codes RENAME TO YEAR_RANGE_CODES;</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C86">
+    <sortCondition ref="A2:A86"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>